<commit_message>
checking functionality and updating excel
</commit_message>
<xml_diff>
--- a/examples/data.xlsx
+++ b/examples/data.xlsx
@@ -5,17 +5,21 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomford/Code/rust-tomlparse/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomford/Code/nvmbuilder/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCBFCAC-91AA-A844-B7BC-9DDD1BB92659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA1E6EA-F9BB-F949-84AA-F48C1C078463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15100" yWindow="760" windowWidth="15140" windowHeight="18880" activeTab="1" xr2:uid="{7DE5358D-EB7B-2445-85B8-580B8690A605}"/>
+    <workbookView xWindow="15100" yWindow="760" windowWidth="15140" windowHeight="18880" xr2:uid="{7DE5358D-EB7B-2445-85B8-580B8690A605}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
-    <sheet name="Normal" sheetId="2" r:id="rId2"/>
-    <sheet name="VarA" sheetId="3" r:id="rId3"/>
+    <sheet name="DefaultCoefficients" sheetId="4" r:id="rId2"/>
+    <sheet name="DebugCoefficients" sheetId="5" r:id="rId3"/>
+    <sheet name="CalibrationMatrix" sheetId="6" r:id="rId4"/>
+    <sheet name="StructArray" sheetId="7" r:id="rId5"/>
+    <sheet name="AnArray" sheetId="8" r:id="rId6"/>
+    <sheet name="Thresholds" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -58,13 +62,112 @@
     <t>Array</t>
   </si>
   <si>
-    <t>Normal</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>DeviceName</t>
+  </si>
+  <si>
+    <t>A Device</t>
+  </si>
+  <si>
+    <t>A Variant</t>
+  </si>
+  <si>
+    <t>SerialNumber</t>
+  </si>
+  <si>
+    <t>FWVersionMajor</t>
+  </si>
+  <si>
+    <t>FWVersionMinor</t>
+  </si>
+  <si>
+    <t>FWVersionPatch</t>
+  </si>
+  <si>
+    <t>WiFiSSID</t>
+  </si>
+  <si>
+    <t>mynetworkname</t>
+  </si>
+  <si>
+    <t>WiFiKey</t>
+  </si>
+  <si>
+    <t>averyveryverylongstring</t>
+  </si>
+  <si>
+    <t>Coefficients1D</t>
+  </si>
+  <si>
+    <t>DefaultCoefficients</t>
+  </si>
+  <si>
+    <t>DebugCoefficients</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>StructArray</t>
+  </si>
+  <si>
+    <t>The rest of these will get padded out</t>
+  </si>
+  <si>
+    <t>Keep comments at least one line away from the table</t>
+  </si>
+  <si>
+    <t>AnArray</t>
+  </si>
+  <si>
+    <t>Block2Description</t>
+  </si>
+  <si>
+    <t>A default descripton</t>
+  </si>
+  <si>
+    <t>A debug description</t>
+  </si>
+  <si>
+    <t>BootCount</t>
+  </si>
+  <si>
+    <t>TemperatureMin</t>
+  </si>
+  <si>
+    <t>TemperatureMax</t>
+  </si>
+  <si>
+    <t>VoltageThresholds</t>
+  </si>
+  <si>
+    <t>Thresholds</t>
+  </si>
+  <si>
+    <t>LegalNotice</t>
+  </si>
+  <si>
+    <t>Don't steal me!</t>
+  </si>
+  <si>
+    <t>CalibrationMatrix</t>
+  </si>
+  <si>
+    <t>AStructs</t>
   </si>
 </sst>
 </file>
@@ -444,48 +547,454 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81175D9F-030E-4648-B932-899D2D945A10}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>100600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22">
+        <v>100</v>
+      </c>
+      <c r="D22">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <v>-30</v>
+      </c>
+      <c r="C23">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <v>50</v>
+      </c>
+      <c r="C24">
+        <v>60</v>
+      </c>
+      <c r="D24">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D3322D-BF46-7347-8CBD-55E083687702}">
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69978073-623F-6244-A16C-3C3F7B61FBCB}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308DF289-3F51-0D46-B1D3-E8F6B2D4D4A5}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6C0CD32-AF17-5A4B-BB00-77BE99ACD882}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>3</v>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -493,22 +1002,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEFA656-A223-384F-8EA2-44D940595C71}">
-  <dimension ref="A1:B10"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D9001E8-18B4-604F-9A9E-44A18637F391}">
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="A11:B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -516,7 +1025,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -524,7 +1033,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -532,7 +1041,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -540,7 +1049,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -548,7 +1057,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -556,7 +1065,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -564,7 +1073,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -572,7 +1081,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -580,7 +1089,15 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -588,62 +1105,39 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB4AD98-D4A0-814A-8F01-4E6F92326AB4}">
-  <dimension ref="A1:B6"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A4B35A9-70FF-A04D-A61F-E1056E9B410A}">
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>11.11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>33.33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>55.55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
+        <v>77.77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Expanded on examples (#4)
* Add block definitions with device, network, and calibration data

Co-authored-by: tfordy63 <tfordy63@gmail.com>

* Add nested structures, 2D arrays, and complex data types to examples

Co-authored-by: tfordy63 <tfordy63@gmail.com>

* checking functionality and updating excel

---------

Co-authored-by: Cursor Agent <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/examples/data.xlsx
+++ b/examples/data.xlsx
@@ -5,17 +5,21 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomford/Code/rust-tomlparse/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomford/Code/nvmbuilder/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCBFCAC-91AA-A844-B7BC-9DDD1BB92659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA1E6EA-F9BB-F949-84AA-F48C1C078463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15100" yWindow="760" windowWidth="15140" windowHeight="18880" activeTab="1" xr2:uid="{7DE5358D-EB7B-2445-85B8-580B8690A605}"/>
+    <workbookView xWindow="15100" yWindow="760" windowWidth="15140" windowHeight="18880" xr2:uid="{7DE5358D-EB7B-2445-85B8-580B8690A605}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
-    <sheet name="Normal" sheetId="2" r:id="rId2"/>
-    <sheet name="VarA" sheetId="3" r:id="rId3"/>
+    <sheet name="DefaultCoefficients" sheetId="4" r:id="rId2"/>
+    <sheet name="DebugCoefficients" sheetId="5" r:id="rId3"/>
+    <sheet name="CalibrationMatrix" sheetId="6" r:id="rId4"/>
+    <sheet name="StructArray" sheetId="7" r:id="rId5"/>
+    <sheet name="AnArray" sheetId="8" r:id="rId6"/>
+    <sheet name="Thresholds" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -58,13 +62,112 @@
     <t>Array</t>
   </si>
   <si>
-    <t>Normal</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>DeviceName</t>
+  </si>
+  <si>
+    <t>A Device</t>
+  </si>
+  <si>
+    <t>A Variant</t>
+  </si>
+  <si>
+    <t>SerialNumber</t>
+  </si>
+  <si>
+    <t>FWVersionMajor</t>
+  </si>
+  <si>
+    <t>FWVersionMinor</t>
+  </si>
+  <si>
+    <t>FWVersionPatch</t>
+  </si>
+  <si>
+    <t>WiFiSSID</t>
+  </si>
+  <si>
+    <t>mynetworkname</t>
+  </si>
+  <si>
+    <t>WiFiKey</t>
+  </si>
+  <si>
+    <t>averyveryverylongstring</t>
+  </si>
+  <si>
+    <t>Coefficients1D</t>
+  </si>
+  <si>
+    <t>DefaultCoefficients</t>
+  </si>
+  <si>
+    <t>DebugCoefficients</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>StructArray</t>
+  </si>
+  <si>
+    <t>The rest of these will get padded out</t>
+  </si>
+  <si>
+    <t>Keep comments at least one line away from the table</t>
+  </si>
+  <si>
+    <t>AnArray</t>
+  </si>
+  <si>
+    <t>Block2Description</t>
+  </si>
+  <si>
+    <t>A default descripton</t>
+  </si>
+  <si>
+    <t>A debug description</t>
+  </si>
+  <si>
+    <t>BootCount</t>
+  </si>
+  <si>
+    <t>TemperatureMin</t>
+  </si>
+  <si>
+    <t>TemperatureMax</t>
+  </si>
+  <si>
+    <t>VoltageThresholds</t>
+  </si>
+  <si>
+    <t>Thresholds</t>
+  </si>
+  <si>
+    <t>LegalNotice</t>
+  </si>
+  <si>
+    <t>Don't steal me!</t>
+  </si>
+  <si>
+    <t>CalibrationMatrix</t>
+  </si>
+  <si>
+    <t>AStructs</t>
   </si>
 </sst>
 </file>
@@ -444,48 +547,454 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81175D9F-030E-4648-B932-899D2D945A10}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>100600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22">
+        <v>100</v>
+      </c>
+      <c r="D22">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <v>-30</v>
+      </c>
+      <c r="C23">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <v>50</v>
+      </c>
+      <c r="C24">
+        <v>60</v>
+      </c>
+      <c r="D24">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D3322D-BF46-7347-8CBD-55E083687702}">
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69978073-623F-6244-A16C-3C3F7B61FBCB}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308DF289-3F51-0D46-B1D3-E8F6B2D4D4A5}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6C0CD32-AF17-5A4B-BB00-77BE99ACD882}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>3</v>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -493,22 +1002,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEFA656-A223-384F-8EA2-44D940595C71}">
-  <dimension ref="A1:B10"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D9001E8-18B4-604F-9A9E-44A18637F391}">
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="A11:B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -516,7 +1025,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -524,7 +1033,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -532,7 +1041,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -540,7 +1049,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -548,7 +1057,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -556,7 +1065,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -564,7 +1073,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -572,7 +1081,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -580,7 +1089,15 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -588,62 +1105,39 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB4AD98-D4A0-814A-8F01-4E6F92326AB4}">
-  <dimension ref="A1:B6"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A4B35A9-70FF-A04D-A61F-E1056E9B410A}">
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>11.11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>33.33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>55.55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
+        <v>77.77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
switching to # because of excel rules
</commit_message>
<xml_diff>
--- a/examples/data.xlsx
+++ b/examples/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomford/Code/nvmbuilder/examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomford/code/projects/nvmbuilder/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA1E6EA-F9BB-F949-84AA-F48C1C078463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259C8242-0CD5-C148-8C6D-EEF28A851E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15100" yWindow="760" windowWidth="15140" windowHeight="18880" xr2:uid="{7DE5358D-EB7B-2445-85B8-580B8690A605}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" xr2:uid="{7DE5358D-EB7B-2445-85B8-580B8690A605}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -104,12 +104,6 @@
     <t>Coefficients1D</t>
   </si>
   <si>
-    <t>DefaultCoefficients</t>
-  </si>
-  <si>
-    <t>DebugCoefficients</t>
-  </si>
-  <si>
     <t>Coefficients</t>
   </si>
   <si>
@@ -122,18 +116,12 @@
     <t>z</t>
   </si>
   <si>
-    <t>StructArray</t>
-  </si>
-  <si>
     <t>The rest of these will get padded out</t>
   </si>
   <si>
     <t>Keep comments at least one line away from the table</t>
   </si>
   <si>
-    <t>AnArray</t>
-  </si>
-  <si>
     <t>Block2Description</t>
   </si>
   <si>
@@ -168,6 +156,24 @@
   </si>
   <si>
     <t>AStructs</t>
+  </si>
+  <si>
+    <t>#Thresholds</t>
+  </si>
+  <si>
+    <t>#AnArray</t>
+  </si>
+  <si>
+    <t>#StructArray</t>
+  </si>
+  <si>
+    <t>#CalibrationMatrix</t>
+  </si>
+  <si>
+    <t>#DefaultCoefficients</t>
+  </si>
+  <si>
+    <t>#DebugCoefficients</t>
   </si>
 </sst>
 </file>
@@ -550,7 +556,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -650,26 +656,26 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -677,23 +683,23 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B22">
         <v>100</v>
@@ -704,7 +710,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B23">
         <v>-30</v>
@@ -715,7 +721,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B24">
         <v>50</v>
@@ -729,18 +735,18 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -760,7 +766,7 @@
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -820,7 +826,7 @@
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -860,13 +866,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -925,7 +931,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -994,7 +1000,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1117,7 +1123,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Implement # prefix for sheet references (#43)
* Refactor: Use '@' prefix for sheet references in DataSheet

Co-authored-by: tfordy63 <tfordy63@gmail.com>

* switching to # because of excel rules

---------

Co-authored-by: Cursor Agent <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/examples/data.xlsx
+++ b/examples/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomford/Code/nvmbuilder/examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomford/code/projects/nvmbuilder/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA1E6EA-F9BB-F949-84AA-F48C1C078463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259C8242-0CD5-C148-8C6D-EEF28A851E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15100" yWindow="760" windowWidth="15140" windowHeight="18880" xr2:uid="{7DE5358D-EB7B-2445-85B8-580B8690A605}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" xr2:uid="{7DE5358D-EB7B-2445-85B8-580B8690A605}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -104,12 +104,6 @@
     <t>Coefficients1D</t>
   </si>
   <si>
-    <t>DefaultCoefficients</t>
-  </si>
-  <si>
-    <t>DebugCoefficients</t>
-  </si>
-  <si>
     <t>Coefficients</t>
   </si>
   <si>
@@ -122,18 +116,12 @@
     <t>z</t>
   </si>
   <si>
-    <t>StructArray</t>
-  </si>
-  <si>
     <t>The rest of these will get padded out</t>
   </si>
   <si>
     <t>Keep comments at least one line away from the table</t>
   </si>
   <si>
-    <t>AnArray</t>
-  </si>
-  <si>
     <t>Block2Description</t>
   </si>
   <si>
@@ -168,6 +156,24 @@
   </si>
   <si>
     <t>AStructs</t>
+  </si>
+  <si>
+    <t>#Thresholds</t>
+  </si>
+  <si>
+    <t>#AnArray</t>
+  </si>
+  <si>
+    <t>#StructArray</t>
+  </si>
+  <si>
+    <t>#CalibrationMatrix</t>
+  </si>
+  <si>
+    <t>#DefaultCoefficients</t>
+  </si>
+  <si>
+    <t>#DebugCoefficients</t>
   </si>
 </sst>
 </file>
@@ -550,7 +556,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -650,26 +656,26 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -677,23 +683,23 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B22">
         <v>100</v>
@@ -704,7 +710,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B23">
         <v>-30</v>
@@ -715,7 +721,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B24">
         <v>50</v>
@@ -729,18 +735,18 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -760,7 +766,7 @@
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -820,7 +826,7 @@
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -860,13 +866,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -925,7 +931,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -994,7 +1000,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1117,7 +1123,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>